<commit_message>
made the code for brutefocring a bit fancier
</commit_message>
<xml_diff>
--- a/bruteforcer_stats.xlsx
+++ b/bruteforcer_stats.xlsx
@@ -1,37 +1,69 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="450" yWindow="570" windowWidth="24640" windowHeight="11490"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>uneven_loss</t>
+  </si>
+  <si>
+    <t>holes_punishment</t>
+  </si>
+  <si>
+    <t>height_diff_punishment</t>
+  </si>
+  <si>
+    <t>attack_bonus</t>
+  </si>
+  <si>
+    <t>max_height_punishment</t>
+  </si>
+  <si>
+    <t>lines_cleared</t>
+  </si>
+  <si>
+    <t>total_attack</t>
+  </si>
+  <si>
+    <t>seed</t>
+  </si>
+  <si>
+    <t>attack_per_line</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +78,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,238 +399,361 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>uneven_loss</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>holes_punishment</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>height_diff_punishment</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>attack_bonus</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>max_height_punishment</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>lines_cleared</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>total_attack</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>seed</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>attack_per_line</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
         <v>0.4</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>0.05</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:9">
+      <c r="A3">
         <v>0.4</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>0.05</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>21</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>12</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>4043354410</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3">
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:9">
+      <c r="A4">
         <v>0.4</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>0.05</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>28</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>9</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>3429245615</v>
       </c>
-      <c r="I4" t="n">
-        <v>0.3214285714285715</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
+      <c r="I4">
+        <v>0.32142857142857151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
         <v>0.4</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>0.05</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>36</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>13</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5">
         <v>1905716920</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5">
         <v>0.3611111111111111</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:9">
+      <c r="A6">
         <v>0.4</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>0.05</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>38</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>20</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>2448336050</v>
       </c>
-      <c r="I6" t="n">
-        <v>0.5263157894736842</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
+      <c r="I6">
+        <v>0.52631578947368418</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
         <v>0.4</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>0.05</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>79</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>35</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>1747751755</v>
       </c>
-      <c r="I7" t="n">
-        <v>0.4430379746835443</v>
+      <c r="I7">
+        <v>0.44303797468354428</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>43.005524376499423</v>
+      </c>
+      <c r="B8">
+        <v>126.8941284988159</v>
+      </c>
+      <c r="C8">
+        <v>3.9004863116698818</v>
+      </c>
+      <c r="D8">
+        <v>174.02038428896179</v>
+      </c>
+      <c r="E8">
+        <v>95.876563404139659</v>
+      </c>
+      <c r="F8">
+        <v>172</v>
+      </c>
+      <c r="G8">
+        <v>67</v>
+      </c>
+      <c r="H8">
+        <v>7575180</v>
+      </c>
+      <c r="I8">
+        <v>0.38953488372093031</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>127.3731032793123</v>
+      </c>
+      <c r="B9">
+        <v>165.16730163234101</v>
+      </c>
+      <c r="C9">
+        <v>48.323113442763521</v>
+      </c>
+      <c r="D9">
+        <v>176.66215411493641</v>
+      </c>
+      <c r="E9">
+        <v>103.5124093744467</v>
+      </c>
+      <c r="F9">
+        <v>225</v>
+      </c>
+      <c r="G9">
+        <v>65</v>
+      </c>
+      <c r="H9">
+        <v>852419985</v>
+      </c>
+      <c r="I9">
+        <v>0.28888888888888892</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>76.086813907099611</v>
+      </c>
+      <c r="B10">
+        <v>197.9220608738149</v>
+      </c>
+      <c r="C10">
+        <v>65.778376403543433</v>
+      </c>
+      <c r="D10">
+        <v>58.916608365085857</v>
+      </c>
+      <c r="E10">
+        <v>59.105473182653668</v>
+      </c>
+      <c r="F10">
+        <v>317</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+      <c r="H10">
+        <v>1063703315</v>
+      </c>
+      <c r="I10">
+        <v>0.31545741324921128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>131.48213576147819</v>
+      </c>
+      <c r="B11">
+        <v>175.12515632096111</v>
+      </c>
+      <c r="C11">
+        <v>11.86954253028296</v>
+      </c>
+      <c r="D11">
+        <v>154.85110615866961</v>
+      </c>
+      <c r="E11">
+        <v>32.443373254533348</v>
+      </c>
+      <c r="F11">
+        <v>559</v>
+      </c>
+      <c r="G11">
+        <v>212</v>
+      </c>
+      <c r="H11">
+        <v>648621800</v>
+      </c>
+      <c r="I11">
+        <v>0.37924865831842569</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>76.192392752049656</v>
+      </c>
+      <c r="B12">
+        <v>167.8227671546498</v>
+      </c>
+      <c r="C12">
+        <v>31.13508109194234</v>
+      </c>
+      <c r="D12">
+        <v>186.69157566085661</v>
+      </c>
+      <c r="E12">
+        <v>67.871516025369942</v>
+      </c>
+      <c r="F12">
+        <v>1291</v>
+      </c>
+      <c r="G12">
+        <v>491</v>
+      </c>
+      <c r="H12">
+        <v>2049559360</v>
+      </c>
+      <c r="I12">
+        <v>0.38032532920216888</v>
       </c>
     </row>
   </sheetData>

</xml_diff>